<commit_message>
Search box added to admin
</commit_message>
<xml_diff>
--- a/OpenGovCore/data/raw_data/old_loksabha_data.xlsx
+++ b/OpenGovCore/data/raw_data/old_loksabha_data.xlsx
@@ -13885,8 +13885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M1133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
-      <selection activeCell="D328" sqref="D328"/>
+    <sheetView tabSelected="1" topLeftCell="A1024" workbookViewId="0">
+      <selection activeCell="D897" sqref="D897"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>